<commit_message>
put together new scaling experiment
</commit_message>
<xml_diff>
--- a/Report/plots/perf_data.xlsx
+++ b/Report/plots/perf_data.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
   <si>
     <t>N</t>
   </si>
@@ -99,6 +99,12 @@
   </si>
   <si>
     <t>efficiency</t>
+  </si>
+  <si>
+    <t>N = 3840</t>
+  </si>
+  <si>
+    <t>N = 7680</t>
   </si>
 </sst>
 </file>
@@ -2336,10 +2342,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2352,6 +2358,9 @@
       <c r="A1" t="s">
         <v>19</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="D1" t="s">
         <v>20</v>
       </c>
@@ -2572,6 +2581,142 @@
       <c r="C13" s="5">
         <f t="shared" si="1"/>
         <v>6.7089009877867936</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1628927133144</v>
+      </c>
+      <c r="C17" s="5">
+        <f>$B$17/B17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18" s="1">
+        <v>875899735704</v>
+      </c>
+      <c r="C18" s="5">
+        <f>$B$17/B18</f>
+        <v>1.8597187175022469</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1">
+        <v>452355152308</v>
+      </c>
+      <c r="C19" s="5">
+        <f>$B$17/B19</f>
+        <v>3.6009916651394622</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>327365800187</v>
+      </c>
+      <c r="C20" s="5">
+        <f>$B$17/B20</f>
+        <v>4.9758622684883811</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1">
+        <v>254374423524</v>
+      </c>
+      <c r="C21" s="5">
+        <f>$B$17/B21</f>
+        <v>6.4036592617194161</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>10</v>
+      </c>
+      <c r="B22" s="1">
+        <v>231848527750</v>
+      </c>
+      <c r="C22" s="5">
+        <f>$B$17/B22</f>
+        <v>7.0258247872095883</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1">
+        <v>220340724398</v>
+      </c>
+      <c r="C23" s="5">
+        <f>$B$17/B23</f>
+        <v>7.3927647174367985</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24" s="1">
+        <v>237683005100</v>
+      </c>
+      <c r="C24" s="5">
+        <f>$B$17/B24</f>
+        <v>6.8533597194240459</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1">
+        <v>218365048581</v>
+      </c>
+      <c r="C25" s="5">
+        <f>$B$17/B25</f>
+        <v>7.459651366962091</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" s="1">
+        <v>226347044864</v>
+      </c>
+      <c r="C26" s="5">
+        <f>$B$17/B26</f>
+        <v>7.1965911201656567</v>
       </c>
     </row>
   </sheetData>
@@ -2741,7 +2886,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2754,6 +2899,9 @@
       <c r="A1" t="s">
         <v>19</v>
       </c>
+      <c r="B1" s="1">
+        <v>3840</v>
+      </c>
       <c r="D1" t="s">
         <v>20</v>
       </c>

</xml_diff>

<commit_message>
finished ADI roofline, worked on report background
</commit_message>
<xml_diff>
--- a/Report/plots/perf_data.xlsx
+++ b/Report/plots/perf_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ADI_serial" sheetId="1" r:id="rId1"/>
@@ -456,20 +456,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
     <col min="3" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="8.5703125"/>
-    <col min="9" max="13" width="8.7109375"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="9.42578125" customWidth="1"/>
+    <col min="10" max="11" width="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.7109375"/>
     <col min="14" max="14" width="10.42578125" customWidth="1"/>
     <col min="15" max="1025" width="8.5703125"/>
   </cols>
@@ -558,15 +560,15 @@
         <v>940</v>
       </c>
       <c r="L2" s="3">
-        <f t="shared" ref="L2:L11" si="5">$F2/(I2*64/10)</f>
+        <f>$F2/(I2*64/10)</f>
         <v>38.730158730158728</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:M11" si="6">$F2/(J2*64/10)</f>
+        <f t="shared" ref="M2:M11" si="5">$F2/(J2*64/10)</f>
         <v>77.529232333502804</v>
       </c>
       <c r="N2" s="3">
-        <f t="shared" ref="N2:N11" si="7">$F2/(K2*64/10)</f>
+        <f t="shared" ref="N2:N11" si="6">$F2/(K2*64/10)</f>
         <v>324.468085106383</v>
       </c>
     </row>
@@ -610,15 +612,15 @@
         <v>977</v>
       </c>
       <c r="L3" s="3">
+        <f t="shared" ref="L2:L11" si="7">$F3/(I3*64/10)</f>
+        <v>139.27576601671308</v>
+      </c>
+      <c r="M3" s="3">
         <f t="shared" si="5"/>
-        <v>139.27576601671308</v>
-      </c>
-      <c r="M3" s="3">
+        <v>319.3663771078181</v>
+      </c>
+      <c r="N3" s="3">
         <f t="shared" si="6"/>
-        <v>319.3663771078181</v>
-      </c>
-      <c r="N3" s="3">
-        <f t="shared" si="7"/>
         <v>1279.4268167860798</v>
       </c>
     </row>
@@ -662,15 +664,15 @@
         <v>946</v>
       </c>
       <c r="L4" s="3">
+        <f t="shared" si="7"/>
+        <v>283.29880745758919</v>
+      </c>
+      <c r="M4" s="3">
         <f t="shared" si="5"/>
-        <v>283.29880745758919</v>
-      </c>
-      <c r="M4" s="3">
+        <v>1040.7239819004526</v>
+      </c>
+      <c r="N4" s="3">
         <f t="shared" si="6"/>
-        <v>1040.7239819004526</v>
-      </c>
-      <c r="N4" s="3">
-        <f t="shared" si="7"/>
         <v>5348.8372093023263</v>
       </c>
     </row>
@@ -714,15 +716,15 @@
         <v>982</v>
       </c>
       <c r="L5" s="3">
+        <f t="shared" si="7"/>
+        <v>1.0171124168494363</v>
+      </c>
+      <c r="M5" s="3">
         <f t="shared" si="5"/>
-        <v>1.0171124168494363</v>
-      </c>
-      <c r="M5" s="3">
+        <v>3515.8003798998443</v>
+      </c>
+      <c r="N5" s="3">
         <f t="shared" si="6"/>
-        <v>3515.8003798998443</v>
-      </c>
-      <c r="N5" s="3">
-        <f t="shared" si="7"/>
         <v>20733.197556008145</v>
       </c>
     </row>
@@ -766,15 +768,15 @@
         <v>983</v>
       </c>
       <c r="L6" s="3">
+        <f t="shared" si="7"/>
+        <v>0.7966485862492716</v>
+      </c>
+      <c r="M6" s="3">
         <f t="shared" si="5"/>
-        <v>0.7966485862492716</v>
-      </c>
-      <c r="M6" s="3">
+        <v>173.09779331966718</v>
+      </c>
+      <c r="N6" s="3">
         <f t="shared" si="6"/>
-        <v>173.09779331966718</v>
-      </c>
-      <c r="N6" s="3">
-        <f t="shared" si="7"/>
         <v>73016.276703967451</v>
       </c>
     </row>
@@ -818,15 +820,15 @@
         <v>1526</v>
       </c>
       <c r="L7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.11297619452733153</v>
+      </c>
+      <c r="M7" s="3">
         <f t="shared" si="5"/>
-        <v>0.11297619452733153</v>
-      </c>
-      <c r="M7" s="3">
+        <v>1.4442106256866374</v>
+      </c>
+      <c r="N7" s="3">
         <f t="shared" si="6"/>
-        <v>1.4442106256866374</v>
-      </c>
-      <c r="N7" s="3">
-        <f t="shared" si="7"/>
         <v>188433.81389252949</v>
       </c>
     </row>
@@ -870,15 +872,15 @@
         <v>1163</v>
       </c>
       <c r="L8" s="3">
+        <f t="shared" si="7"/>
+        <v>0.13902928857192301</v>
+      </c>
+      <c r="M8" s="3">
         <f t="shared" si="5"/>
-        <v>0.13902928857192301</v>
-      </c>
-      <c r="M8" s="3">
+        <v>0.37857981065600621</v>
+      </c>
+      <c r="N8" s="3">
         <f t="shared" si="6"/>
-        <v>0.37857981065600621</v>
-      </c>
-      <c r="N8" s="3">
-        <f t="shared" si="7"/>
         <v>989767.84178847808</v>
       </c>
     </row>
@@ -922,15 +924,15 @@
         <v>287681</v>
       </c>
       <c r="L9" s="3">
+        <f t="shared" si="7"/>
+        <v>0.1109471858798966</v>
+      </c>
+      <c r="M9" s="3">
         <f t="shared" si="5"/>
-        <v>0.1109471858798966</v>
-      </c>
-      <c r="M9" s="3">
+        <v>0.6294274614911799</v>
+      </c>
+      <c r="N9" s="3">
         <f t="shared" si="6"/>
-        <v>0.6294274614911799</v>
-      </c>
-      <c r="N9" s="3">
-        <f t="shared" si="7"/>
         <v>16011.484943392161</v>
       </c>
     </row>
@@ -974,15 +976,15 @@
         <v>7893370650</v>
       </c>
       <c r="L10" s="3">
+        <f t="shared" si="7"/>
+        <v>9.4924798542548497E-2</v>
+      </c>
+      <c r="M10" s="3">
         <f t="shared" si="5"/>
-        <v>9.4924798542548497E-2</v>
-      </c>
-      <c r="M10" s="3">
+        <v>0.13211342271344223</v>
+      </c>
+      <c r="N10" s="3">
         <f t="shared" si="6"/>
-        <v>0.13211342271344223</v>
-      </c>
-      <c r="N10" s="3">
-        <f t="shared" si="7"/>
         <v>2.3346680166349465</v>
       </c>
     </row>
@@ -1026,15 +1028,15 @@
         <v>38542235695</v>
       </c>
       <c r="L11" s="3">
+        <f t="shared" si="7"/>
+        <v>7.48897216596148E-2</v>
+      </c>
+      <c r="M11" s="3">
         <f t="shared" si="5"/>
-        <v>7.48897216596148E-2</v>
-      </c>
-      <c r="M11" s="3">
+        <v>0.11106209539007619</v>
+      </c>
+      <c r="N11" s="3">
         <f t="shared" si="6"/>
-        <v>0.11106209539007619</v>
-      </c>
-      <c r="N11" s="3">
-        <f t="shared" si="7"/>
         <v>1.9127276524221879</v>
       </c>
     </row>
@@ -1042,7 +1044,7 @@
       <c r="A12">
         <v>7682</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <v>1000</v>
       </c>
       <c r="C12" s="1">
@@ -1068,22 +1070,31 @@
         <f t="shared" si="4"/>
         <v>0.27424815382317891</v>
       </c>
-      <c r="L12" s="3" t="e">
+      <c r="I12" s="1">
+        <v>3528229359318</v>
+      </c>
+      <c r="J12" s="1">
+        <v>2491589212433</v>
+      </c>
+      <c r="K12" s="1">
+        <v>151962447726</v>
+      </c>
+      <c r="L12" s="3">
         <f t="shared" ref="L12" si="8">$F12/(I12*64/10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="3" t="e">
+        <v>8.358232131966703E-2</v>
+      </c>
+      <c r="M12" s="3">
         <f t="shared" ref="M12" si="9">$F12/(J12*64/10)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" s="3" t="e">
+        <v>0.11835723101082014</v>
+      </c>
+      <c r="N12" s="3">
         <f t="shared" ref="N12" si="10">$F12/(K12*64/10)</f>
-        <v>#DIV/0!</v>
+        <v>1.9405952221283187</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1095,25 +1106,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="1" customWidth="1"/>
     <col min="4" max="5" width="8.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.42578125" style="1"/>
-    <col min="7" max="7" width="8.5703125"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
     <col min="8" max="8" width="8.28515625"/>
     <col min="9" max="9" width="7.140625"/>
     <col min="10" max="10" width="9.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.42578125" style="1" customWidth="1"/>
     <col min="12" max="12" width="9" style="1" customWidth="1"/>
     <col min="13" max="14" width="8.5703125"/>
-    <col min="15" max="15" width="9.7109375"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
     <col min="16" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
@@ -1208,16 +1219,16 @@
         <v>922</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:M11" si="6">$E2/(J2*64)</f>
-        <v>1.9603934077618288</v>
+        <f>$E2/(J2*64/10)</f>
+        <v>19.603934077618288</v>
       </c>
       <c r="N2" s="3">
-        <f t="shared" ref="N2:N11" si="7">$E2/(K2*64)</f>
-        <v>3.9735991379310347</v>
+        <f>$E2/(K2*64/10)</f>
+        <v>39.735991379310349</v>
       </c>
       <c r="O2" s="3">
-        <f t="shared" ref="O2:O11" si="8">$E2/(L2*64)</f>
-        <v>15.997830802603037</v>
+        <f t="shared" ref="N2:O12" si="6">$E2/(L2*64/10)</f>
+        <v>159.97830802603036</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -1264,16 +1275,16 @@
         <v>1007</v>
       </c>
       <c r="M3" s="3">
+        <f t="shared" ref="M3:M12" si="7">$E3/(J3*64/10)</f>
+        <v>63.430777716492003</v>
+      </c>
+      <c r="N3" s="3">
         <f t="shared" si="6"/>
-        <v>6.3430777716492006</v>
-      </c>
-      <c r="N3" s="3">
-        <f t="shared" si="7"/>
-        <v>14.131236175964611</v>
+        <v>141.31236175964611</v>
       </c>
       <c r="O3" s="3">
-        <f t="shared" si="8"/>
-        <v>57.100297914597817</v>
+        <f t="shared" si="6"/>
+        <v>571.00297914597809</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1320,16 +1331,16 @@
         <v>1017</v>
       </c>
       <c r="M4" s="3">
+        <f t="shared" si="7"/>
+        <v>26.669486348042671</v>
+      </c>
+      <c r="N4" s="3">
         <f t="shared" si="6"/>
-        <v>2.666948634804267</v>
-      </c>
-      <c r="N4" s="3">
-        <f t="shared" si="7"/>
-        <v>48.339011925042591</v>
+        <v>483.39011925042587</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="8"/>
-        <v>223.20550639134709</v>
+        <f t="shared" si="6"/>
+        <v>2232.0550639134708</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1376,16 +1387,16 @@
         <v>1022</v>
       </c>
       <c r="M5" s="3">
+        <f t="shared" si="7"/>
+        <v>0.43094171035605006</v>
+      </c>
+      <c r="N5" s="3">
         <f t="shared" si="6"/>
-        <v>4.3094171035605006E-2</v>
-      </c>
-      <c r="N5" s="3">
-        <f t="shared" si="7"/>
-        <v>117.8314826910516</v>
+        <v>1178.3148269105161</v>
       </c>
       <c r="O5" s="3">
-        <f t="shared" si="8"/>
-        <v>882.58317025440317</v>
+        <f t="shared" si="6"/>
+        <v>8825.8317025440319</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1432,16 +1443,16 @@
         <v>1061</v>
       </c>
       <c r="M6" s="3">
+        <f t="shared" si="7"/>
+        <v>0.24405173262139165</v>
+      </c>
+      <c r="N6" s="3">
         <f t="shared" si="6"/>
-        <v>2.4405173262139167E-2</v>
-      </c>
-      <c r="N6" s="3">
-        <f t="shared" si="7"/>
-        <v>0.91375510351555445</v>
+        <v>9.1375510351555445</v>
       </c>
       <c r="O6" s="3">
-        <f t="shared" si="8"/>
-        <v>2979.5004712535342</v>
+        <f t="shared" si="6"/>
+        <v>29795.004712535345</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1488,16 +1499,16 @@
         <v>1052</v>
       </c>
       <c r="M7" s="3">
+        <f t="shared" si="7"/>
+        <v>0.15932003237605205</v>
+      </c>
+      <c r="N7" s="3">
         <f t="shared" si="6"/>
-        <v>1.5932003237605203E-2</v>
-      </c>
-      <c r="N7" s="3">
-        <f t="shared" si="7"/>
-        <v>5.7897075828202707E-2</v>
+        <v>0.57897075828202704</v>
       </c>
       <c r="O7" s="3">
-        <f t="shared" si="8"/>
-        <v>11998.574144486693</v>
+        <f t="shared" si="6"/>
+        <v>119985.74144486692</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1544,16 +1555,16 @@
         <v>1216</v>
       </c>
       <c r="M8" s="3">
+        <f t="shared" si="7"/>
+        <v>0.15104254631658376</v>
+      </c>
+      <c r="N8" s="3">
         <f t="shared" si="6"/>
-        <v>1.5104254631658376E-2</v>
-      </c>
-      <c r="N8" s="3">
-        <f t="shared" si="7"/>
-        <v>3.8880280388627723E-2</v>
+        <v>0.38880280388627719</v>
       </c>
       <c r="O8" s="3">
-        <f t="shared" si="8"/>
-        <v>41484.375</v>
+        <f t="shared" si="6"/>
+        <v>414843.75</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1600,16 +1611,16 @@
         <v>809193</v>
       </c>
       <c r="M9" s="3">
+        <f t="shared" si="7"/>
+        <v>0.14349313910151162</v>
+      </c>
+      <c r="N9" s="3">
         <f t="shared" si="6"/>
-        <v>1.4349313910151162E-2</v>
-      </c>
-      <c r="N9" s="3">
-        <f t="shared" si="7"/>
-        <v>2.7458757729395582E-2</v>
+        <v>0.27458757729395583</v>
       </c>
       <c r="O9" s="3">
-        <f t="shared" si="8"/>
-        <v>249.24832518323811</v>
+        <f t="shared" si="6"/>
+        <v>2492.483251832381</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1656,16 +1667,16 @@
         <v>7789079598</v>
       </c>
       <c r="M10" s="3">
+        <f t="shared" si="7"/>
+        <v>0.13669033802728073</v>
+      </c>
+      <c r="N10" s="3">
         <f t="shared" si="6"/>
-        <v>1.3669033802728072E-2</v>
-      </c>
-      <c r="N10" s="3">
-        <f t="shared" si="7"/>
-        <v>2.2130262783050452E-2</v>
+        <v>0.22130262783050453</v>
       </c>
       <c r="O10" s="3">
-        <f t="shared" si="8"/>
-        <v>0.10355267138457609</v>
+        <f t="shared" si="6"/>
+        <v>1.0355267138457609</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1712,16 +1723,16 @@
         <v>38520460874</v>
       </c>
       <c r="M11" s="3">
+        <f t="shared" si="7"/>
+        <v>0.12464892844004291</v>
+      </c>
+      <c r="N11" s="3">
         <f t="shared" si="6"/>
-        <v>1.2464892844004292E-2</v>
-      </c>
-      <c r="N11" s="3">
-        <f t="shared" si="7"/>
-        <v>2.0003180250563423E-2</v>
+        <v>0.20003180250563424</v>
       </c>
       <c r="O11" s="3">
-        <f t="shared" si="8"/>
-        <v>8.3746661561295427E-2</v>
+        <f t="shared" si="6"/>
+        <v>0.83746661561295421</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1758,22 +1769,31 @@
         <f t="shared" si="5"/>
         <v>0.18216278527099214</v>
       </c>
-      <c r="M12" s="3" t="e">
-        <f t="shared" ref="M12" si="9">$E12/(J12*64)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N12" s="3" t="e">
-        <f t="shared" ref="N12" si="10">$E12/(K12*64)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O12" s="3" t="e">
-        <f t="shared" ref="O12" si="11">$E12/(L12*64)</f>
-        <v>#DIV/0!</v>
+      <c r="J12" s="1">
+        <v>1162706322942</v>
+      </c>
+      <c r="K12" s="1">
+        <v>762121984961</v>
+      </c>
+      <c r="L12" s="1">
+        <v>153303507648</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="7"/>
+        <v>0.11097488458952549</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="6"/>
+        <v>0.16930518020235683</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="6"/>
+        <v>0.8416715441127961</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1785,22 +1805,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" style="1" customWidth="1"/>
     <col min="3" max="5" width="9.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="1"/>
-    <col min="7" max="7" width="8.5703125"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="9.28515625" customWidth="1"/>
-    <col min="11" max="12" width="8.5703125"/>
-    <col min="13" max="13" width="10.140625"/>
+    <col min="11" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" customWidth="1"/>
     <col min="14" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
@@ -1881,16 +1901,16 @@
         <v>943</v>
       </c>
       <c r="K2" s="3">
-        <f t="shared" ref="K2:K11" si="4">$E2/(H2*64)</f>
-        <v>2.0229468599033815</v>
+        <f>$E2/(H2*64/10)</f>
+        <v>20.229468599033815</v>
       </c>
       <c r="L2" s="3">
-        <f t="shared" ref="L2:L11" si="5">$E2/(I2*64)</f>
-        <v>4.3859649122807021</v>
+        <f t="shared" ref="L2:M12" si="4">$E2/(I2*64/10)</f>
+        <v>43.859649122807021</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" ref="M2:M11" si="6">$E2/(J2*64)</f>
-        <v>17.762460233297986</v>
+        <f t="shared" si="4"/>
+        <v>177.62460233297986</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -1929,16 +1949,16 @@
         <v>1047</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" si="4"/>
-        <v>7.2866837245522307</v>
+        <f t="shared" ref="K3:K12" si="5">$E3/(H3*64/10)</f>
+        <v>72.866837245522305</v>
       </c>
       <c r="L3" s="3">
-        <f t="shared" si="5"/>
-        <v>13.859500634786288</v>
+        <f t="shared" si="4"/>
+        <v>138.59500634786289</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" si="6"/>
-        <v>62.559694364851957</v>
+        <f t="shared" si="4"/>
+        <v>625.59694364851953</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1977,16 +1997,16 @@
         <v>1009</v>
       </c>
       <c r="K4" s="3">
-        <f t="shared" si="4"/>
-        <v>11.218920557913886</v>
+        <f t="shared" si="5"/>
+        <v>112.18920557913887</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="5"/>
-        <v>49.258273107645493</v>
+        <f t="shared" si="4"/>
+        <v>492.58273107645499</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="6"/>
-        <v>256.6897918731417</v>
+        <f t="shared" si="4"/>
+        <v>2566.8979187314171</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -2025,16 +2045,16 @@
         <v>1022</v>
       </c>
       <c r="K5" s="3">
-        <f t="shared" si="4"/>
-        <v>4.9869789012542833E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.49869789012542837</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="5"/>
-        <v>146.74455050577006</v>
+        <f t="shared" si="4"/>
+        <v>1467.4455050577005</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="6"/>
-        <v>1007.8277886497065</v>
+        <f t="shared" si="4"/>
+        <v>10078.277886497064</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -2073,16 +2093,16 @@
         <v>1008</v>
       </c>
       <c r="K6" s="3">
-        <f t="shared" si="4"/>
-        <v>2.8001085166596395E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.28001085166596396</v>
       </c>
       <c r="L6" s="3">
-        <f t="shared" si="5"/>
-        <v>0.41094959769328826</v>
+        <f t="shared" si="4"/>
+        <v>4.1094959769328829</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="6"/>
-        <v>3582.5892857142858</v>
+        <f t="shared" si="4"/>
+        <v>35825.892857142855</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -2121,16 +2141,16 @@
         <v>1075</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" si="4"/>
-        <v>1.9315341488373855E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.19315341488373855</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="5"/>
-        <v>6.8079428048026691E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.68079428048026691</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="6"/>
-        <v>13416.279069767443</v>
+        <f t="shared" si="4"/>
+        <v>134162.79069767441</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -2169,16 +2189,16 @@
         <v>2165</v>
       </c>
       <c r="K8" s="3">
-        <f t="shared" si="4"/>
-        <v>1.8522076546094651E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.18522076546094648</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="5"/>
-        <v>6.309754211107467E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.63097542111074667</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="6"/>
-        <v>26625.866050808316</v>
+        <f t="shared" si="4"/>
+        <v>266258.66050808312</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -2217,16 +2237,16 @@
         <v>1064463</v>
       </c>
       <c r="K9" s="3">
-        <f t="shared" si="4"/>
-        <v>1.7371827263261461E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.17371827263261461</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="5"/>
-        <v>3.630064167623262E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.36300641676232615</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" si="6"/>
-        <v>216.53171599200724</v>
+        <f t="shared" si="4"/>
+        <v>2165.3171599200723</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -2265,16 +2285,16 @@
         <v>7733202693</v>
       </c>
       <c r="K10" s="3">
-        <f t="shared" si="4"/>
-        <v>1.6467803046771683E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.16467803046771684</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" si="5"/>
-        <v>2.7444327600431903E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.274443276004319</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" si="6"/>
-        <v>0.11919770327944254</v>
+        <f t="shared" si="4"/>
+        <v>1.1919770327944255</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -2313,16 +2333,16 @@
         <v>37848264041</v>
       </c>
       <c r="K11" s="3">
-        <f t="shared" si="4"/>
-        <v>1.5120894161249822E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.15120894161249823</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="5"/>
-        <v>2.4638059969106597E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.24638059969106599</v>
       </c>
       <c r="M11" s="3">
-        <f t="shared" si="6"/>
-        <v>9.7408958994955025E-2</v>
+        <f t="shared" si="4"/>
+        <v>0.97408958994955031</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -2351,22 +2371,31 @@
         <f t="shared" si="3"/>
         <v>0.80124549028609748</v>
       </c>
-      <c r="K12" s="3" t="e">
-        <f t="shared" ref="K12" si="7">$E12/(H12*64)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L12" s="3" t="e">
-        <f t="shared" ref="L12" si="8">$E12/(I12*64)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M12" s="3" t="e">
-        <f t="shared" ref="M12" si="9">$E12/(J12*64)</f>
-        <v>#DIV/0!</v>
+      <c r="H12" s="1">
+        <v>1053733191403</v>
+      </c>
+      <c r="I12" s="1">
+        <v>669488703078</v>
+      </c>
+      <c r="J12" s="1">
+        <v>153182807373</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="5"/>
+        <v>0.13994358458392978</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="4"/>
+        <v>0.22026241715809733</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="4"/>
+        <v>0.96266155797058373</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2849,10 +2878,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3007,6 +3036,9 @@
       <c r="D11" s="6">
         <v>728742030923</v>
       </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="C16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>